<commit_message>
Added Replacer_mapping for ISPResults
</commit_message>
<xml_diff>
--- a/src/exso/Files/ReportsInfo.xlsx
+++ b/src/exso/Files/ReportsInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanos\Desktop\Admie-Desktop\exso\src\exso\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.natsikas\Desktop\Admie-Desktop\exso\src\exso\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A26A29B-1103-40E1-9913-4B29302DB7BC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B47CEA3-3FB3-4B40-AE0D-49E0AFC096E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Parse Settings'!$A$1:$F$76</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Read Settings'!$A$1:$H$76</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -751,19 +763,10 @@
     </comment>
     <comment ref="A20" authorId="1" shapeId="0" xr:uid="{D125AC30-4B70-4B9E-BF83-3DD2FAF1754D}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     one of the files is .xls instead of xlsx, so I add ad-hoc eligibiltiy file to include it (somewhere in April 2021)</t>
-        </r>
       </text>
     </comment>
     <comment ref="E98" authorId="0" shapeId="0" xr:uid="{F0F1C47D-4F5B-4B9D-9AD3-8B6711A5850E}">
@@ -1020,19 +1023,10 @@
     </comment>
     <comment ref="F2" authorId="1" shapeId="0" xr:uid="{9954997E-FE91-4A98-940C-46F8F94F700E}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     not really, but will be handled in the Parsers</t>
-        </r>
       </text>
     </comment>
     <comment ref="E26" authorId="0" shapeId="0" xr:uid="{C165D3FC-00A9-4540-AF8C-5B218DA01CBE}">
@@ -1103,36 +1097,18 @@
     </comment>
     <comment ref="E89" authorId="2" shapeId="0" xr:uid="{C40E5BBA-8535-41A3-90E8-3B8469C6238D}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     SYSTEM SCADA IS EET. I know it fom inside</t>
-        </r>
       </text>
     </comment>
     <comment ref="E90" authorId="3" shapeId="0" xr:uid="{1EAC3B27-A1A4-4877-BCC3-D0F826980256}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     SYSTEM SCADA IS EET. I know it fom inside</t>
-        </r>
       </text>
     </comment>
     <comment ref="E93" authorId="0" shapeId="0" xr:uid="{587BE131-561E-4065-AB0B-6DB901C9B2DF}">
@@ -1163,19 +1139,10 @@
     </comment>
     <comment ref="E98" authorId="4" shapeId="0" xr:uid="{CF4C0D3B-5669-4C09-AB25-32B5B39E7391}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     SYSTEM SCADA IS EET. I know it fom inside</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -1183,7 +1150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="313">
   <si>
     <t>AdhocISPResults</t>
   </si>
@@ -2123,6 +2090,9 @@
   </si>
   <si>
     <t>ISPForecasts</t>
+  </si>
+  <si>
+    <t>ISPResults.csv</t>
   </si>
 </sst>
 </file>
@@ -2702,7 +2672,35 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="514">
+  <dxfs count="518">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6644,7 +6642,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D71" sqref="D71:D72"/>
     </sheetView>
   </sheetViews>
@@ -10089,739 +10087,739 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K108" xr:uid="{8D662490-7F15-44D9-82E3-9F132913C8FA}"/>
-  <sortState ref="A2:J108">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J108">
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="B2:B113">
-    <cfRule type="expression" dxfId="513" priority="270">
+    <cfRule type="expression" dxfId="517" priority="270">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B113">
-    <cfRule type="expression" dxfId="512" priority="271">
+    <cfRule type="expression" dxfId="516" priority="271">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="expression" dxfId="511" priority="269">
+    <cfRule type="expression" dxfId="515" priority="269">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="expression" dxfId="510" priority="268">
+    <cfRule type="expression" dxfId="514" priority="268">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" dxfId="509" priority="267">
+    <cfRule type="expression" dxfId="513" priority="267">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="508" priority="266">
+    <cfRule type="expression" dxfId="512" priority="266">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="expression" dxfId="507" priority="265">
+    <cfRule type="expression" dxfId="511" priority="265">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="expression" dxfId="506" priority="264">
+    <cfRule type="expression" dxfId="510" priority="264">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91:B105">
-    <cfRule type="expression" dxfId="505" priority="263">
+    <cfRule type="expression" dxfId="509" priority="263">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79:B81">
-    <cfRule type="expression" dxfId="504" priority="262">
+    <cfRule type="expression" dxfId="508" priority="262">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="503" priority="261">
+    <cfRule type="expression" dxfId="507" priority="261">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="expression" dxfId="502" priority="260">
+    <cfRule type="expression" dxfId="506" priority="260">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" dxfId="501" priority="259">
+    <cfRule type="expression" dxfId="505" priority="259">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="500" priority="258">
+    <cfRule type="expression" dxfId="504" priority="258">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="expression" dxfId="499" priority="257">
+    <cfRule type="expression" dxfId="503" priority="257">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F79 E112:F113 E82:F106">
-    <cfRule type="expression" dxfId="498" priority="200">
+    <cfRule type="expression" dxfId="502" priority="200">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:F79 E112:F113 E82:F106">
-    <cfRule type="expression" dxfId="497" priority="201">
+    <cfRule type="expression" dxfId="501" priority="201">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80:F80">
-    <cfRule type="expression" dxfId="496" priority="198">
+    <cfRule type="expression" dxfId="500" priority="198">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80:F80">
-    <cfRule type="expression" dxfId="495" priority="199">
+    <cfRule type="expression" dxfId="499" priority="199">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81">
-    <cfRule type="expression" dxfId="494" priority="196">
+    <cfRule type="expression" dxfId="498" priority="196">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81">
-    <cfRule type="expression" dxfId="493" priority="197">
+    <cfRule type="expression" dxfId="497" priority="197">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="expression" dxfId="492" priority="194">
+    <cfRule type="expression" dxfId="496" priority="194">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="expression" dxfId="491" priority="195">
+    <cfRule type="expression" dxfId="495" priority="195">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107:F112">
-    <cfRule type="expression" dxfId="490" priority="192">
+    <cfRule type="expression" dxfId="494" priority="192">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107:F112">
-    <cfRule type="expression" dxfId="489" priority="193">
+    <cfRule type="expression" dxfId="493" priority="193">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A113">
-    <cfRule type="expression" dxfId="488" priority="124">
+    <cfRule type="expression" dxfId="492" priority="124">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A113">
-    <cfRule type="expression" dxfId="487" priority="125">
+    <cfRule type="expression" dxfId="491" priority="125">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="expression" dxfId="486" priority="123">
+    <cfRule type="expression" dxfId="490" priority="123">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="485" priority="122">
+    <cfRule type="expression" dxfId="489" priority="122">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="484" priority="121">
+    <cfRule type="expression" dxfId="488" priority="121">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="483" priority="120">
+    <cfRule type="expression" dxfId="487" priority="120">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="482" priority="119">
+    <cfRule type="expression" dxfId="486" priority="119">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="481" priority="118">
+    <cfRule type="expression" dxfId="485" priority="118">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:A105">
-    <cfRule type="expression" dxfId="480" priority="117">
+    <cfRule type="expression" dxfId="484" priority="117">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79:A81">
-    <cfRule type="expression" dxfId="479" priority="116">
+    <cfRule type="expression" dxfId="483" priority="116">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="478" priority="115">
+    <cfRule type="expression" dxfId="482" priority="115">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="477" priority="114">
+    <cfRule type="expression" dxfId="481" priority="114">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="476" priority="113">
+    <cfRule type="expression" dxfId="480" priority="113">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="475" priority="112">
+    <cfRule type="expression" dxfId="479" priority="112">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="474" priority="111">
+    <cfRule type="expression" dxfId="478" priority="111">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C113">
-    <cfRule type="expression" dxfId="473" priority="109">
+    <cfRule type="expression" dxfId="477" priority="109">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C113">
-    <cfRule type="expression" dxfId="472" priority="110">
+    <cfRule type="expression" dxfId="476" priority="110">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
-    <cfRule type="expression" dxfId="471" priority="108">
+    <cfRule type="expression" dxfId="475" priority="108">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="expression" dxfId="470" priority="107">
+    <cfRule type="expression" dxfId="474" priority="107">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="expression" dxfId="469" priority="106">
+    <cfRule type="expression" dxfId="473" priority="106">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="expression" dxfId="468" priority="105">
+    <cfRule type="expression" dxfId="472" priority="105">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92">
-    <cfRule type="expression" dxfId="467" priority="104">
+    <cfRule type="expression" dxfId="471" priority="104">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="expression" dxfId="466" priority="103">
+    <cfRule type="expression" dxfId="470" priority="103">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91:C105">
-    <cfRule type="expression" dxfId="465" priority="102">
+    <cfRule type="expression" dxfId="469" priority="102">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79:C81">
-    <cfRule type="expression" dxfId="464" priority="101">
+    <cfRule type="expression" dxfId="468" priority="101">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88">
-    <cfRule type="expression" dxfId="463" priority="100">
+    <cfRule type="expression" dxfId="467" priority="100">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="expression" dxfId="462" priority="99">
+    <cfRule type="expression" dxfId="466" priority="99">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="expression" dxfId="461" priority="98">
+    <cfRule type="expression" dxfId="465" priority="98">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="expression" dxfId="460" priority="97">
+    <cfRule type="expression" dxfId="464" priority="97">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92">
-    <cfRule type="expression" dxfId="459" priority="96">
+    <cfRule type="expression" dxfId="463" priority="96">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D113">
-    <cfRule type="expression" dxfId="458" priority="94">
+    <cfRule type="expression" dxfId="462" priority="94">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D113">
-    <cfRule type="expression" dxfId="457" priority="95">
+    <cfRule type="expression" dxfId="461" priority="95">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="expression" dxfId="456" priority="93">
+    <cfRule type="expression" dxfId="460" priority="93">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89">
-    <cfRule type="expression" dxfId="455" priority="92">
+    <cfRule type="expression" dxfId="459" priority="92">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D90">
-    <cfRule type="expression" dxfId="454" priority="91">
+    <cfRule type="expression" dxfId="458" priority="91">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D91">
-    <cfRule type="expression" dxfId="453" priority="90">
+    <cfRule type="expression" dxfId="457" priority="90">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="expression" dxfId="452" priority="89">
+    <cfRule type="expression" dxfId="456" priority="89">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="expression" dxfId="451" priority="88">
+    <cfRule type="expression" dxfId="455" priority="88">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D91:D105">
-    <cfRule type="expression" dxfId="450" priority="87">
+    <cfRule type="expression" dxfId="454" priority="87">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79:D81">
-    <cfRule type="expression" dxfId="449" priority="86">
+    <cfRule type="expression" dxfId="453" priority="86">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88">
-    <cfRule type="expression" dxfId="448" priority="85">
+    <cfRule type="expression" dxfId="452" priority="85">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89">
-    <cfRule type="expression" dxfId="447" priority="84">
+    <cfRule type="expression" dxfId="451" priority="84">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D90">
-    <cfRule type="expression" dxfId="446" priority="83">
+    <cfRule type="expression" dxfId="450" priority="83">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D91">
-    <cfRule type="expression" dxfId="445" priority="82">
+    <cfRule type="expression" dxfId="449" priority="82">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="expression" dxfId="444" priority="81">
+    <cfRule type="expression" dxfId="448" priority="81">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G113">
-    <cfRule type="expression" dxfId="443" priority="79">
+    <cfRule type="expression" dxfId="447" priority="79">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G113">
-    <cfRule type="expression" dxfId="442" priority="80">
+    <cfRule type="expression" dxfId="446" priority="80">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G78">
-    <cfRule type="expression" dxfId="441" priority="78">
+    <cfRule type="expression" dxfId="445" priority="78">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G89">
-    <cfRule type="expression" dxfId="440" priority="77">
+    <cfRule type="expression" dxfId="444" priority="77">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G90">
-    <cfRule type="expression" dxfId="439" priority="76">
+    <cfRule type="expression" dxfId="443" priority="76">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91">
-    <cfRule type="expression" dxfId="438" priority="75">
+    <cfRule type="expression" dxfId="442" priority="75">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G92">
-    <cfRule type="expression" dxfId="437" priority="74">
+    <cfRule type="expression" dxfId="441" priority="74">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G93">
-    <cfRule type="expression" dxfId="436" priority="73">
+    <cfRule type="expression" dxfId="440" priority="73">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91:G105">
-    <cfRule type="expression" dxfId="435" priority="72">
+    <cfRule type="expression" dxfId="439" priority="72">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:G81">
-    <cfRule type="expression" dxfId="434" priority="71">
+    <cfRule type="expression" dxfId="438" priority="71">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88">
-    <cfRule type="expression" dxfId="433" priority="70">
+    <cfRule type="expression" dxfId="437" priority="70">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G89">
-    <cfRule type="expression" dxfId="432" priority="69">
+    <cfRule type="expression" dxfId="436" priority="69">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G90">
-    <cfRule type="expression" dxfId="431" priority="68">
+    <cfRule type="expression" dxfId="435" priority="68">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91">
-    <cfRule type="expression" dxfId="430" priority="67">
+    <cfRule type="expression" dxfId="434" priority="67">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G92">
-    <cfRule type="expression" dxfId="429" priority="66">
+    <cfRule type="expression" dxfId="433" priority="66">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H113">
-    <cfRule type="expression" dxfId="428" priority="64">
+    <cfRule type="expression" dxfId="432" priority="64">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H113">
-    <cfRule type="expression" dxfId="427" priority="65">
+    <cfRule type="expression" dxfId="431" priority="65">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="426" priority="63">
+    <cfRule type="expression" dxfId="430" priority="63">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="expression" dxfId="425" priority="62">
+    <cfRule type="expression" dxfId="429" priority="62">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H90">
-    <cfRule type="expression" dxfId="424" priority="61">
+    <cfRule type="expression" dxfId="428" priority="61">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H91">
-    <cfRule type="expression" dxfId="423" priority="60">
+    <cfRule type="expression" dxfId="427" priority="60">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92">
-    <cfRule type="expression" dxfId="422" priority="59">
+    <cfRule type="expression" dxfId="426" priority="59">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H93">
-    <cfRule type="expression" dxfId="421" priority="58">
+    <cfRule type="expression" dxfId="425" priority="58">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H91:H105">
-    <cfRule type="expression" dxfId="420" priority="57">
+    <cfRule type="expression" dxfId="424" priority="57">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79:H81">
-    <cfRule type="expression" dxfId="419" priority="56">
+    <cfRule type="expression" dxfId="423" priority="56">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="expression" dxfId="418" priority="55">
+    <cfRule type="expression" dxfId="422" priority="55">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="expression" dxfId="417" priority="54">
+    <cfRule type="expression" dxfId="421" priority="54">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H90">
-    <cfRule type="expression" dxfId="416" priority="53">
+    <cfRule type="expression" dxfId="420" priority="53">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H91">
-    <cfRule type="expression" dxfId="415" priority="52">
+    <cfRule type="expression" dxfId="419" priority="52">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92">
-    <cfRule type="expression" dxfId="414" priority="51">
+    <cfRule type="expression" dxfId="418" priority="51">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J113">
-    <cfRule type="expression" dxfId="413" priority="49">
+    <cfRule type="expression" dxfId="417" priority="49">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J113">
-    <cfRule type="expression" dxfId="412" priority="50">
+    <cfRule type="expression" dxfId="416" priority="50">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J78">
-    <cfRule type="expression" dxfId="411" priority="48">
+    <cfRule type="expression" dxfId="415" priority="48">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J89">
-    <cfRule type="expression" dxfId="410" priority="47">
+    <cfRule type="expression" dxfId="414" priority="47">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J90">
-    <cfRule type="expression" dxfId="409" priority="46">
+    <cfRule type="expression" dxfId="413" priority="46">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J91">
-    <cfRule type="expression" dxfId="408" priority="45">
+    <cfRule type="expression" dxfId="412" priority="45">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92">
-    <cfRule type="expression" dxfId="407" priority="44">
+    <cfRule type="expression" dxfId="411" priority="44">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J93">
-    <cfRule type="expression" dxfId="406" priority="43">
+    <cfRule type="expression" dxfId="410" priority="43">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J91:J105">
-    <cfRule type="expression" dxfId="405" priority="42">
+    <cfRule type="expression" dxfId="409" priority="42">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J79:J81">
-    <cfRule type="expression" dxfId="404" priority="41">
+    <cfRule type="expression" dxfId="408" priority="41">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88">
-    <cfRule type="expression" dxfId="403" priority="40">
+    <cfRule type="expression" dxfId="407" priority="40">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J89">
-    <cfRule type="expression" dxfId="402" priority="39">
+    <cfRule type="expression" dxfId="406" priority="39">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J90">
-    <cfRule type="expression" dxfId="401" priority="38">
+    <cfRule type="expression" dxfId="405" priority="38">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J91">
-    <cfRule type="expression" dxfId="400" priority="37">
+    <cfRule type="expression" dxfId="404" priority="37">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92">
-    <cfRule type="expression" dxfId="399" priority="36">
+    <cfRule type="expression" dxfId="403" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I113">
-    <cfRule type="cellIs" dxfId="398" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="402" priority="33" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="397" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="32" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K113">
-    <cfRule type="expression" dxfId="396" priority="29">
+    <cfRule type="expression" dxfId="400" priority="29">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K113">
-    <cfRule type="expression" dxfId="395" priority="30">
+    <cfRule type="expression" dxfId="399" priority="30">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78">
-    <cfRule type="expression" dxfId="394" priority="28">
+    <cfRule type="expression" dxfId="398" priority="28">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K89">
-    <cfRule type="expression" dxfId="393" priority="27">
+    <cfRule type="expression" dxfId="397" priority="27">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K90">
-    <cfRule type="expression" dxfId="392" priority="26">
+    <cfRule type="expression" dxfId="396" priority="26">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K91">
-    <cfRule type="expression" dxfId="391" priority="25">
+    <cfRule type="expression" dxfId="395" priority="25">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92">
-    <cfRule type="expression" dxfId="390" priority="24">
+    <cfRule type="expression" dxfId="394" priority="24">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K93">
-    <cfRule type="expression" dxfId="389" priority="23">
+    <cfRule type="expression" dxfId="393" priority="23">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K91:K105">
-    <cfRule type="expression" dxfId="388" priority="22">
+    <cfRule type="expression" dxfId="392" priority="22">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K79:K81">
-    <cfRule type="expression" dxfId="387" priority="21">
+    <cfRule type="expression" dxfId="391" priority="21">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88">
-    <cfRule type="expression" dxfId="386" priority="20">
+    <cfRule type="expression" dxfId="390" priority="20">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K89">
-    <cfRule type="expression" dxfId="385" priority="19">
+    <cfRule type="expression" dxfId="389" priority="19">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K90">
-    <cfRule type="expression" dxfId="384" priority="18">
+    <cfRule type="expression" dxfId="388" priority="18">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K91">
-    <cfRule type="expression" dxfId="383" priority="17">
+    <cfRule type="expression" dxfId="387" priority="17">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92">
-    <cfRule type="expression" dxfId="382" priority="16">
+    <cfRule type="expression" dxfId="386" priority="16">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89">
-    <cfRule type="expression" dxfId="381" priority="15">
+    <cfRule type="expression" dxfId="385" priority="15">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89">
-    <cfRule type="expression" dxfId="380" priority="14">
+    <cfRule type="expression" dxfId="384" priority="14">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="expression" dxfId="379" priority="13">
+    <cfRule type="expression" dxfId="383" priority="13">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="expression" dxfId="378" priority="12">
+    <cfRule type="expression" dxfId="382" priority="12">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="expression" dxfId="377" priority="11">
+    <cfRule type="expression" dxfId="381" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="expression" dxfId="376" priority="10">
+    <cfRule type="expression" dxfId="380" priority="10">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="expression" dxfId="375" priority="9">
+    <cfRule type="expression" dxfId="379" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="expression" dxfId="374" priority="8">
+    <cfRule type="expression" dxfId="378" priority="8">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="expression" dxfId="373" priority="7">
+    <cfRule type="expression" dxfId="377" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="expression" dxfId="372" priority="6">
+    <cfRule type="expression" dxfId="376" priority="6">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98">
-    <cfRule type="expression" dxfId="371" priority="5">
+    <cfRule type="expression" dxfId="375" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98">
-    <cfRule type="expression" dxfId="370" priority="4">
+    <cfRule type="expression" dxfId="374" priority="4">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98">
-    <cfRule type="expression" dxfId="369" priority="3">
+    <cfRule type="expression" dxfId="373" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98">
-    <cfRule type="expression" dxfId="368" priority="2">
+    <cfRule type="expression" dxfId="372" priority="2">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D82">
-    <cfRule type="expression" dxfId="367" priority="1">
+    <cfRule type="expression" dxfId="371" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12851,546 +12849,546 @@
       <c r="H113" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:H108">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H108">
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="E100:E108 E34:F34 E38:F38 E42:F42 E46:F46 E50:F50 E54:F54 E55:H63 G82:H108 E35:H37 E39:H41 E43:H45 E47:H49 E51:H53 A109:H113 H69 E70:H73 E75:F99 G75:H79 H74 E65:H68 E64 G64:H64 E2:H33">
-    <cfRule type="expression" dxfId="366" priority="202">
+    <cfRule type="expression" dxfId="370" priority="202">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E100:E108 E34:F34 E38:F38 E42:F42 E46:F46 E50:F50 E54:F54 E55:H63 G82:H108 A1:H1 E35:H37 E39:H41 E43:H45 E47:H49 E51:H53 A109:H113 H69 E70:H73 E75:F99 G75:H79 H74 E65:H68 E64 G64:H64 E2:H33">
-    <cfRule type="expression" dxfId="365" priority="203">
+    <cfRule type="expression" dxfId="369" priority="203">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="expression" dxfId="364" priority="194">
+    <cfRule type="expression" dxfId="368" priority="194">
       <formula>OR(ROW()=CELL("row"),COL()=CELL("col"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:D109">
-    <cfRule type="expression" dxfId="363" priority="167">
+    <cfRule type="expression" dxfId="367" priority="167">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G80:H80 G81">
-    <cfRule type="expression" dxfId="362" priority="150">
+    <cfRule type="expression" dxfId="366" priority="150">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G80:H80 G81">
-    <cfRule type="expression" dxfId="361" priority="151">
+    <cfRule type="expression" dxfId="365" priority="151">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="360" priority="142">
+    <cfRule type="expression" dxfId="364" priority="142">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="359" priority="143">
+    <cfRule type="expression" dxfId="363" priority="143">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F100:F108">
-    <cfRule type="expression" dxfId="358" priority="136">
+    <cfRule type="expression" dxfId="362" priority="136">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F100:F108">
-    <cfRule type="expression" dxfId="357" priority="137">
+    <cfRule type="expression" dxfId="361" priority="137">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77:D77">
-    <cfRule type="expression" dxfId="356" priority="111">
+    <cfRule type="expression" dxfId="360" priority="111">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84:D84">
-    <cfRule type="expression" dxfId="355" priority="109">
+    <cfRule type="expression" dxfId="359" priority="109">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86:D86">
-    <cfRule type="expression" dxfId="354" priority="107">
+    <cfRule type="expression" dxfId="358" priority="107">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78:D78">
-    <cfRule type="expression" dxfId="353" priority="105">
+    <cfRule type="expression" dxfId="357" priority="105">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D22 D3:D113 B23:D23 A24:D108">
-    <cfRule type="expression" dxfId="352" priority="112">
+    <cfRule type="expression" dxfId="356" priority="112">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D22 D3:D113 B23:D23 A24:D108">
-    <cfRule type="expression" dxfId="351" priority="113">
+    <cfRule type="expression" dxfId="355" priority="113">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79:D83">
-    <cfRule type="expression" dxfId="350" priority="110">
+    <cfRule type="expression" dxfId="354" priority="110">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:D85">
-    <cfRule type="expression" dxfId="349" priority="108">
+    <cfRule type="expression" dxfId="353" priority="108">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:D88">
-    <cfRule type="expression" dxfId="348" priority="106">
+    <cfRule type="expression" dxfId="352" priority="106">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89:D89">
-    <cfRule type="expression" dxfId="347" priority="104">
+    <cfRule type="expression" dxfId="351" priority="104">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:D90">
-    <cfRule type="expression" dxfId="346" priority="103">
+    <cfRule type="expression" dxfId="350" priority="103">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:D91">
-    <cfRule type="expression" dxfId="345" priority="102">
+    <cfRule type="expression" dxfId="349" priority="102">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:D92">
-    <cfRule type="expression" dxfId="344" priority="101">
+    <cfRule type="expression" dxfId="348" priority="101">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:D93">
-    <cfRule type="expression" dxfId="343" priority="100">
+    <cfRule type="expression" dxfId="347" priority="100">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94:D94">
-    <cfRule type="expression" dxfId="342" priority="99">
+    <cfRule type="expression" dxfId="346" priority="99">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:D95">
-    <cfRule type="expression" dxfId="341" priority="98">
+    <cfRule type="expression" dxfId="345" priority="98">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:D96">
-    <cfRule type="expression" dxfId="340" priority="97">
+    <cfRule type="expression" dxfId="344" priority="97">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97:D97">
-    <cfRule type="expression" dxfId="339" priority="96">
+    <cfRule type="expression" dxfId="343" priority="96">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:D98">
-    <cfRule type="expression" dxfId="338" priority="95">
+    <cfRule type="expression" dxfId="342" priority="95">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:D99">
-    <cfRule type="expression" dxfId="337" priority="94">
+    <cfRule type="expression" dxfId="341" priority="94">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:D100">
-    <cfRule type="expression" dxfId="336" priority="93">
+    <cfRule type="expression" dxfId="340" priority="93">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:D101">
-    <cfRule type="expression" dxfId="335" priority="92">
+    <cfRule type="expression" dxfId="339" priority="92">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:D102">
-    <cfRule type="expression" dxfId="334" priority="91">
+    <cfRule type="expression" dxfId="338" priority="91">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103:D103">
-    <cfRule type="expression" dxfId="333" priority="90">
+    <cfRule type="expression" dxfId="337" priority="90">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104:D104">
-    <cfRule type="expression" dxfId="332" priority="89">
+    <cfRule type="expression" dxfId="336" priority="89">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:D105">
-    <cfRule type="expression" dxfId="331" priority="88">
+    <cfRule type="expression" dxfId="335" priority="88">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106:D106">
-    <cfRule type="expression" dxfId="330" priority="87">
+    <cfRule type="expression" dxfId="334" priority="87">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107:D107">
-    <cfRule type="expression" dxfId="329" priority="86">
+    <cfRule type="expression" dxfId="333" priority="86">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108:D108">
-    <cfRule type="expression" dxfId="328" priority="85">
+    <cfRule type="expression" dxfId="332" priority="85">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:D83">
-    <cfRule type="expression" dxfId="327" priority="84">
+    <cfRule type="expression" dxfId="331" priority="84">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84:D84">
-    <cfRule type="expression" dxfId="326" priority="83">
+    <cfRule type="expression" dxfId="330" priority="83">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:D85">
-    <cfRule type="expression" dxfId="325" priority="82">
+    <cfRule type="expression" dxfId="329" priority="82">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86:D86">
-    <cfRule type="expression" dxfId="324" priority="81">
+    <cfRule type="expression" dxfId="328" priority="81">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:D88">
-    <cfRule type="expression" dxfId="323" priority="80">
+    <cfRule type="expression" dxfId="327" priority="80">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89:D89">
-    <cfRule type="expression" dxfId="322" priority="79">
+    <cfRule type="expression" dxfId="326" priority="79">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:D90">
-    <cfRule type="expression" dxfId="321" priority="78">
+    <cfRule type="expression" dxfId="325" priority="78">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:D91">
-    <cfRule type="expression" dxfId="320" priority="77">
+    <cfRule type="expression" dxfId="324" priority="77">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:D92">
-    <cfRule type="expression" dxfId="319" priority="76">
+    <cfRule type="expression" dxfId="323" priority="76">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:D93">
-    <cfRule type="expression" dxfId="318" priority="75">
+    <cfRule type="expression" dxfId="322" priority="75">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94:D94">
-    <cfRule type="expression" dxfId="317" priority="74">
+    <cfRule type="expression" dxfId="321" priority="74">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:D95">
-    <cfRule type="expression" dxfId="316" priority="73">
+    <cfRule type="expression" dxfId="320" priority="73">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:D96">
-    <cfRule type="expression" dxfId="315" priority="72">
+    <cfRule type="expression" dxfId="319" priority="72">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97:D97">
-    <cfRule type="expression" dxfId="314" priority="71">
+    <cfRule type="expression" dxfId="318" priority="71">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:D98">
-    <cfRule type="expression" dxfId="313" priority="70">
+    <cfRule type="expression" dxfId="317" priority="70">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:D99">
-    <cfRule type="expression" dxfId="312" priority="69">
+    <cfRule type="expression" dxfId="316" priority="69">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:D100">
-    <cfRule type="expression" dxfId="311" priority="68">
+    <cfRule type="expression" dxfId="315" priority="68">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:D101">
-    <cfRule type="expression" dxfId="310" priority="67">
+    <cfRule type="expression" dxfId="314" priority="67">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:D102">
-    <cfRule type="expression" dxfId="309" priority="66">
+    <cfRule type="expression" dxfId="313" priority="66">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103:D103">
-    <cfRule type="expression" dxfId="308" priority="65">
+    <cfRule type="expression" dxfId="312" priority="65">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104:D104">
-    <cfRule type="expression" dxfId="307" priority="64">
+    <cfRule type="expression" dxfId="311" priority="64">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:D105">
-    <cfRule type="expression" dxfId="306" priority="63">
+    <cfRule type="expression" dxfId="310" priority="63">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:D100">
-    <cfRule type="expression" dxfId="305" priority="62">
+    <cfRule type="expression" dxfId="309" priority="62">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:D101">
-    <cfRule type="expression" dxfId="304" priority="61">
+    <cfRule type="expression" dxfId="308" priority="61">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:D102">
-    <cfRule type="expression" dxfId="303" priority="60">
+    <cfRule type="expression" dxfId="307" priority="60">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103:D103">
-    <cfRule type="expression" dxfId="302" priority="59">
+    <cfRule type="expression" dxfId="306" priority="59">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104:D104">
-    <cfRule type="expression" dxfId="301" priority="58">
+    <cfRule type="expression" dxfId="305" priority="58">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:D105">
-    <cfRule type="expression" dxfId="300" priority="57">
+    <cfRule type="expression" dxfId="304" priority="57">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:H34">
-    <cfRule type="expression" dxfId="299" priority="40">
+    <cfRule type="expression" dxfId="303" priority="40">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:H34">
-    <cfRule type="expression" dxfId="298" priority="41">
+    <cfRule type="expression" dxfId="302" priority="41">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38:H38">
-    <cfRule type="expression" dxfId="297" priority="38">
+    <cfRule type="expression" dxfId="301" priority="38">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38:H38">
-    <cfRule type="expression" dxfId="296" priority="39">
+    <cfRule type="expression" dxfId="300" priority="39">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:H42">
-    <cfRule type="expression" dxfId="295" priority="36">
+    <cfRule type="expression" dxfId="299" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:H42">
-    <cfRule type="expression" dxfId="294" priority="37">
+    <cfRule type="expression" dxfId="298" priority="37">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46:H46">
-    <cfRule type="expression" dxfId="293" priority="34">
+    <cfRule type="expression" dxfId="297" priority="34">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46:H46">
-    <cfRule type="expression" dxfId="292" priority="35">
+    <cfRule type="expression" dxfId="296" priority="35">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50:H50">
-    <cfRule type="expression" dxfId="291" priority="32">
+    <cfRule type="expression" dxfId="295" priority="32">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50:H50">
-    <cfRule type="expression" dxfId="290" priority="33">
+    <cfRule type="expression" dxfId="294" priority="33">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54:H54">
-    <cfRule type="expression" dxfId="289" priority="30">
+    <cfRule type="expression" dxfId="293" priority="30">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54:H54">
-    <cfRule type="expression" dxfId="288" priority="31">
+    <cfRule type="expression" dxfId="292" priority="31">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D116">
-    <cfRule type="expression" dxfId="287" priority="28">
+    <cfRule type="expression" dxfId="291" priority="28">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D116">
-    <cfRule type="expression" dxfId="286" priority="29">
+    <cfRule type="expression" dxfId="290" priority="29">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89:D89">
-    <cfRule type="expression" dxfId="285" priority="27">
+    <cfRule type="expression" dxfId="289" priority="27">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90:D90">
-    <cfRule type="expression" dxfId="284" priority="26">
+    <cfRule type="expression" dxfId="288" priority="26">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91:D91">
-    <cfRule type="expression" dxfId="283" priority="25">
+    <cfRule type="expression" dxfId="287" priority="25">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92:D92">
-    <cfRule type="expression" dxfId="282" priority="24">
+    <cfRule type="expression" dxfId="286" priority="24">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93:D93">
-    <cfRule type="expression" dxfId="281" priority="23">
+    <cfRule type="expression" dxfId="285" priority="23">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91:D105">
-    <cfRule type="expression" dxfId="280" priority="22">
+    <cfRule type="expression" dxfId="284" priority="22">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:D88">
-    <cfRule type="expression" dxfId="279" priority="21">
+    <cfRule type="expression" dxfId="283" priority="21">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89:D89">
-    <cfRule type="expression" dxfId="278" priority="20">
+    <cfRule type="expression" dxfId="282" priority="20">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90:D90">
-    <cfRule type="expression" dxfId="277" priority="19">
+    <cfRule type="expression" dxfId="281" priority="19">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91:D91">
-    <cfRule type="expression" dxfId="276" priority="18">
+    <cfRule type="expression" dxfId="280" priority="18">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92:D92">
-    <cfRule type="expression" dxfId="275" priority="17">
+    <cfRule type="expression" dxfId="279" priority="17">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:D110">
-    <cfRule type="expression" dxfId="274" priority="16">
+    <cfRule type="expression" dxfId="278" priority="16">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111:D111">
-    <cfRule type="expression" dxfId="273" priority="15">
+    <cfRule type="expression" dxfId="277" priority="15">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69 G69">
-    <cfRule type="expression" dxfId="272" priority="13">
+    <cfRule type="expression" dxfId="276" priority="13">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69 G69">
-    <cfRule type="expression" dxfId="271" priority="14">
+    <cfRule type="expression" dxfId="275" priority="14">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:G74">
-    <cfRule type="expression" dxfId="270" priority="11">
+    <cfRule type="expression" dxfId="274" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:G74">
-    <cfRule type="expression" dxfId="269" priority="12">
+    <cfRule type="expression" dxfId="273" priority="12">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69">
-    <cfRule type="expression" dxfId="268" priority="9">
+    <cfRule type="expression" dxfId="272" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69">
-    <cfRule type="expression" dxfId="267" priority="10">
+    <cfRule type="expression" dxfId="271" priority="10">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
-    <cfRule type="expression" dxfId="266" priority="7">
+    <cfRule type="expression" dxfId="270" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
-    <cfRule type="expression" dxfId="265" priority="8">
+    <cfRule type="expression" dxfId="269" priority="8">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="264" priority="5">
+    <cfRule type="expression" dxfId="268" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="263" priority="6">
+    <cfRule type="expression" dxfId="267" priority="6">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" dxfId="262" priority="4">
+    <cfRule type="expression" dxfId="266" priority="4">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" dxfId="261" priority="3">
+    <cfRule type="expression" dxfId="265" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" dxfId="260" priority="2">
+    <cfRule type="expression" dxfId="264" priority="2">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" dxfId="259" priority="1">
+    <cfRule type="expression" dxfId="263" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13404,8 +13402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D990D66-1D5A-4927-9AF4-58A372472D57}">
   <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13454,7 +13452,9 @@
         <v>111</v>
       </c>
       <c r="C2" s="38"/>
-      <c r="D2" s="22"/>
+      <c r="D2" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="E2" s="22" t="s">
         <v>245</v>
       </c>
@@ -14418,7 +14418,9 @@
         <v>111</v>
       </c>
       <c r="C63" s="38"/>
-      <c r="D63" s="22"/>
+      <c r="D63" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="E63" s="22" t="s">
         <v>245</v>
       </c>
@@ -14498,7 +14500,9 @@
         <v>111</v>
       </c>
       <c r="C68" s="38"/>
-      <c r="D68" s="22"/>
+      <c r="D68" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="E68" s="22" t="s">
         <v>245</v>
       </c>
@@ -14578,7 +14582,9 @@
         <v>111</v>
       </c>
       <c r="C73" s="38"/>
-      <c r="D73" s="22"/>
+      <c r="D73" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="E73" s="22" t="s">
         <v>245</v>
       </c>
@@ -15104,602 +15110,622 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F82:H93 E82:E99 H100:H111 H55:H79 C107:E108 B64:C68 F94:G108 E64:E68 A109:G113 B3:E25 F55:G68 F3:H54 B26:C26 E26 B27:E63 G69 E70:G73 B70:C73 B75:B108 C75:C106 E75:E79 F75:G80 G74 B2:H2">
-    <cfRule type="expression" dxfId="258" priority="133">
+    <cfRule type="expression" dxfId="262" priority="137">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F82:H93 E82:E99 H100:H111 H55:H79 C107:E108 B64:C68 F94:G108 E64:E68 A109:G113 B3:E25 F55:G68 A1:H1 B26:C26 E26 B27:E63 G69 E70:G73 B70:C73 B75:B108 C75:C106 E75:E79 F75:G80 G74 F3:H54 B2:H2">
-    <cfRule type="expression" dxfId="257" priority="134">
+    <cfRule type="expression" dxfId="261" priority="138">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82:B88">
-    <cfRule type="expression" dxfId="256" priority="132">
+    <cfRule type="expression" dxfId="260" priority="136">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:E25">
-    <cfRule type="expression" dxfId="255" priority="131">
+    <cfRule type="expression" dxfId="259" priority="135">
       <formula>OR(ROW()=CELL("row"),COL()=CELL("col"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109">
-    <cfRule type="expression" dxfId="254" priority="130">
+    <cfRule type="expression" dxfId="258" priority="134">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F110:F111 F101:F105">
-    <cfRule type="expression" dxfId="253" priority="129">
+    <cfRule type="expression" dxfId="257" priority="133">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:G81 H80:H81">
-    <cfRule type="expression" dxfId="252" priority="127">
+    <cfRule type="expression" dxfId="256" priority="131">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:G81 H80:H81">
-    <cfRule type="expression" dxfId="251" priority="128">
+    <cfRule type="expression" dxfId="255" priority="132">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80:E81">
-    <cfRule type="expression" dxfId="250" priority="125">
+    <cfRule type="expression" dxfId="254" priority="129">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80:E81">
-    <cfRule type="expression" dxfId="249" priority="126">
+    <cfRule type="expression" dxfId="253" priority="130">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E100:E106">
+    <cfRule type="expression" dxfId="252" priority="125">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E100:E106">
+    <cfRule type="expression" dxfId="251" priority="126">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D82:D99 D64 D66:D67 D71:D72 D76:D79">
+    <cfRule type="expression" dxfId="250" priority="123">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D82:D99 D64 D66:D67 D71:D72 D76:D79">
+    <cfRule type="expression" dxfId="249" priority="124">
+      <formula>COLUMN()=CELL("col")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D80:D81">
     <cfRule type="expression" dxfId="248" priority="121">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E100:E106">
+  <conditionalFormatting sqref="D80:D81">
     <cfRule type="expression" dxfId="247" priority="122">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D82:D99 D64 D66:D68 D71:D73 D76:D79">
+  <conditionalFormatting sqref="D100:D106">
     <cfRule type="expression" dxfId="246" priority="119">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D82:D99 D64 D66:D68 D71:D73 D76:D79">
+  <conditionalFormatting sqref="D100:D106">
     <cfRule type="expression" dxfId="245" priority="120">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D80:D81">
+  <conditionalFormatting sqref="G94">
     <cfRule type="expression" dxfId="244" priority="117">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D80:D81">
+  <conditionalFormatting sqref="G94">
     <cfRule type="expression" dxfId="243" priority="118">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D100:D106">
+  <conditionalFormatting sqref="G95">
     <cfRule type="expression" dxfId="242" priority="115">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D100:D106">
+  <conditionalFormatting sqref="G95">
     <cfRule type="expression" dxfId="241" priority="116">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G94">
+  <conditionalFormatting sqref="G96">
     <cfRule type="expression" dxfId="240" priority="113">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G94">
+  <conditionalFormatting sqref="G96">
     <cfRule type="expression" dxfId="239" priority="114">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G95">
+  <conditionalFormatting sqref="G97">
     <cfRule type="expression" dxfId="238" priority="111">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G95">
+  <conditionalFormatting sqref="G97">
     <cfRule type="expression" dxfId="237" priority="112">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G96">
+  <conditionalFormatting sqref="G98">
     <cfRule type="expression" dxfId="236" priority="109">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G96">
+  <conditionalFormatting sqref="G98">
     <cfRule type="expression" dxfId="235" priority="110">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G97">
+  <conditionalFormatting sqref="G99">
     <cfRule type="expression" dxfId="234" priority="107">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G97">
+  <conditionalFormatting sqref="G99">
     <cfRule type="expression" dxfId="233" priority="108">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G98">
+  <conditionalFormatting sqref="A2:A22 A24:A108">
     <cfRule type="expression" dxfId="232" priority="105">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G98">
+  <conditionalFormatting sqref="A2:A22 A24:A108">
     <cfRule type="expression" dxfId="231" priority="106">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G99">
-    <cfRule type="expression" dxfId="230" priority="103">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G99">
-    <cfRule type="expression" dxfId="229" priority="104">
+  <conditionalFormatting sqref="A77">
+    <cfRule type="expression" dxfId="230" priority="104">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79:A83">
+    <cfRule type="expression" dxfId="229" priority="103">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="expression" dxfId="228" priority="102">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
+    <cfRule type="expression" dxfId="227" priority="101">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86">
+    <cfRule type="expression" dxfId="226" priority="100">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="expression" dxfId="225" priority="99">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78">
+    <cfRule type="expression" dxfId="224" priority="98">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="expression" dxfId="223" priority="97">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="222" priority="96">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="221" priority="95">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="expression" dxfId="220" priority="94">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93">
+    <cfRule type="expression" dxfId="219" priority="93">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="expression" dxfId="218" priority="92">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="expression" dxfId="217" priority="91">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="expression" dxfId="216" priority="90">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="expression" dxfId="215" priority="89">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98">
+    <cfRule type="expression" dxfId="214" priority="88">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A99">
+    <cfRule type="expression" dxfId="213" priority="87">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="expression" dxfId="212" priority="86">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="expression" dxfId="211" priority="85">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102">
+    <cfRule type="expression" dxfId="210" priority="84">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="expression" dxfId="209" priority="83">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="expression" dxfId="208" priority="82">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="expression" dxfId="207" priority="81">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106">
+    <cfRule type="expression" dxfId="206" priority="80">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A107">
+    <cfRule type="expression" dxfId="205" priority="79">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A108">
+    <cfRule type="expression" dxfId="204" priority="78">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83">
+    <cfRule type="expression" dxfId="203" priority="77">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A84">
+    <cfRule type="expression" dxfId="202" priority="76">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
+    <cfRule type="expression" dxfId="201" priority="75">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86">
+    <cfRule type="expression" dxfId="200" priority="74">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="expression" dxfId="199" priority="73">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89">
+    <cfRule type="expression" dxfId="198" priority="72">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="197" priority="71">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="196" priority="70">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="expression" dxfId="195" priority="69">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93">
+    <cfRule type="expression" dxfId="194" priority="68">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A94">
+    <cfRule type="expression" dxfId="193" priority="67">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="expression" dxfId="192" priority="66">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="expression" dxfId="191" priority="65">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="expression" dxfId="190" priority="64">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98">
+    <cfRule type="expression" dxfId="189" priority="63">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A99">
+    <cfRule type="expression" dxfId="188" priority="62">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="expression" dxfId="187" priority="61">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="expression" dxfId="186" priority="60">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102">
+    <cfRule type="expression" dxfId="185" priority="59">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="expression" dxfId="184" priority="58">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="expression" dxfId="183" priority="57">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="expression" dxfId="182" priority="56">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="expression" dxfId="181" priority="55">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="expression" dxfId="180" priority="54">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A102">
+    <cfRule type="expression" dxfId="179" priority="53">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103">
+    <cfRule type="expression" dxfId="178" priority="52">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="expression" dxfId="177" priority="51">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="expression" dxfId="176" priority="50">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G110:G111 G101:G105">
+    <cfRule type="expression" dxfId="175" priority="49">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F81">
+    <cfRule type="expression" dxfId="174" priority="47">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F81">
+    <cfRule type="expression" dxfId="173" priority="48">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A22 A24:A108">
-    <cfRule type="expression" dxfId="228" priority="101">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A22 A24:A108">
-    <cfRule type="expression" dxfId="227" priority="102">
+  <conditionalFormatting sqref="H94">
+    <cfRule type="expression" dxfId="172" priority="45">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H94">
+    <cfRule type="expression" dxfId="171" priority="46">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="expression" dxfId="226" priority="100">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A79:A83">
-    <cfRule type="expression" dxfId="225" priority="99">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="224" priority="98">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="223" priority="97">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="222" priority="96">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="221" priority="95">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A78">
-    <cfRule type="expression" dxfId="220" priority="94">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="219" priority="93">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="218" priority="92">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="217" priority="91">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="216" priority="90">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="215" priority="89">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="214" priority="88">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="213" priority="87">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="212" priority="86">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="211" priority="85">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="210" priority="84">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="209" priority="83">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="208" priority="82">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="207" priority="81">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="206" priority="80">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="205" priority="79">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="204" priority="78">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="203" priority="77">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
-    <cfRule type="expression" dxfId="202" priority="76">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
-    <cfRule type="expression" dxfId="201" priority="75">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A108">
-    <cfRule type="expression" dxfId="200" priority="74">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A83">
-    <cfRule type="expression" dxfId="199" priority="73">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="198" priority="72">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="197" priority="71">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="196" priority="70">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="195" priority="69">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="194" priority="68">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="193" priority="67">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="192" priority="66">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="191" priority="65">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="190" priority="64">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="189" priority="63">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="188" priority="62">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="187" priority="61">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="186" priority="60">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="185" priority="59">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="184" priority="58">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="183" priority="57">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="182" priority="56">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="181" priority="55">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="180" priority="54">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="179" priority="53">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="178" priority="52">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="177" priority="51">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="176" priority="50">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="175" priority="49">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="174" priority="48">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="173" priority="47">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="172" priority="46">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G110:G111 G101:G105">
-    <cfRule type="expression" dxfId="171" priority="45">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F81">
+  <conditionalFormatting sqref="H95">
     <cfRule type="expression" dxfId="170" priority="43">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F81">
+  <conditionalFormatting sqref="H95">
     <cfRule type="expression" dxfId="169" priority="44">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H94">
+  <conditionalFormatting sqref="H96">
     <cfRule type="expression" dxfId="168" priority="41">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H94">
+  <conditionalFormatting sqref="H96">
     <cfRule type="expression" dxfId="167" priority="42">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H95">
+  <conditionalFormatting sqref="H97">
     <cfRule type="expression" dxfId="166" priority="39">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H95">
+  <conditionalFormatting sqref="H97">
     <cfRule type="expression" dxfId="165" priority="40">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H96">
+  <conditionalFormatting sqref="H98">
     <cfRule type="expression" dxfId="164" priority="37">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H96">
+  <conditionalFormatting sqref="H98">
     <cfRule type="expression" dxfId="163" priority="38">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H97">
+  <conditionalFormatting sqref="H99">
     <cfRule type="expression" dxfId="162" priority="35">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H97">
+  <conditionalFormatting sqref="H99">
     <cfRule type="expression" dxfId="161" priority="36">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H98">
-    <cfRule type="expression" dxfId="160" priority="33">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H98">
-    <cfRule type="expression" dxfId="159" priority="34">
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="160" priority="21">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="159" priority="22">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H99">
-    <cfRule type="expression" dxfId="158" priority="31">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H99">
-    <cfRule type="expression" dxfId="157" priority="32">
+  <conditionalFormatting sqref="D70">
+    <cfRule type="expression" dxfId="158" priority="19">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D70">
+    <cfRule type="expression" dxfId="157" priority="20">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
+  <conditionalFormatting sqref="D75">
     <cfRule type="expression" dxfId="156" priority="17">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
+  <conditionalFormatting sqref="D75">
     <cfRule type="expression" dxfId="155" priority="18">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D70">
+  <conditionalFormatting sqref="D26">
     <cfRule type="expression" dxfId="154" priority="15">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D70">
+  <conditionalFormatting sqref="D26">
     <cfRule type="expression" dxfId="153" priority="16">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75">
+  <conditionalFormatting sqref="B69:C69 E69:F69">
     <cfRule type="expression" dxfId="152" priority="13">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75">
+  <conditionalFormatting sqref="B69:C69 E69:F69">
     <cfRule type="expression" dxfId="151" priority="14">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
+  <conditionalFormatting sqref="D69">
     <cfRule type="expression" dxfId="150" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
+  <conditionalFormatting sqref="D69">
     <cfRule type="expression" dxfId="149" priority="12">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69:C69 E69:F69">
+  <conditionalFormatting sqref="B74:C74 E74:F74">
     <cfRule type="expression" dxfId="148" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69:C69 E69:F69">
+  <conditionalFormatting sqref="B74:C74 E74:F74">
     <cfRule type="expression" dxfId="147" priority="10">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D69">
+  <conditionalFormatting sqref="D74">
     <cfRule type="expression" dxfId="146" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D69">
+  <conditionalFormatting sqref="D74">
     <cfRule type="expression" dxfId="145" priority="8">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B74:C74 E74:F74">
+  <conditionalFormatting sqref="A23">
     <cfRule type="expression" dxfId="144" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B74:C74 E74:F74">
+  <conditionalFormatting sqref="A23">
     <cfRule type="expression" dxfId="143" priority="6">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D74">
-    <cfRule type="expression" dxfId="142" priority="3">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D74">
-    <cfRule type="expression" dxfId="141" priority="4">
+  <conditionalFormatting sqref="D68">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="140" priority="1">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="139" priority="2">
+  <conditionalFormatting sqref="D73">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>ROW()=CELL("row")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D73">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17950,371 +17976,371 @@
       <c r="H112" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:J108">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J108">
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A112:H115 B2:H79 B82:H106">
-    <cfRule type="expression" dxfId="138" priority="117">
+    <cfRule type="expression" dxfId="142" priority="117">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:H1 A112:H115 B2:H79 B82:H106">
-    <cfRule type="expression" dxfId="137" priority="118">
+    <cfRule type="expression" dxfId="141" priority="118">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="expression" dxfId="136" priority="83">
+    <cfRule type="expression" dxfId="140" priority="83">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:H80">
-    <cfRule type="expression" dxfId="135" priority="77">
+    <cfRule type="expression" dxfId="139" priority="77">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:H80">
-    <cfRule type="expression" dxfId="134" priority="78">
+    <cfRule type="expression" dxfId="138" priority="78">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81:F81 H81">
-    <cfRule type="expression" dxfId="133" priority="72">
+    <cfRule type="expression" dxfId="137" priority="72">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81:F81 H81">
-    <cfRule type="expression" dxfId="132" priority="73">
+    <cfRule type="expression" dxfId="136" priority="73">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81:C81">
-    <cfRule type="expression" dxfId="131" priority="70">
+    <cfRule type="expression" dxfId="135" priority="70">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81:C81">
-    <cfRule type="expression" dxfId="130" priority="71">
+    <cfRule type="expression" dxfId="134" priority="71">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81">
-    <cfRule type="expression" dxfId="129" priority="68">
+    <cfRule type="expression" dxfId="133" priority="68">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81">
-    <cfRule type="expression" dxfId="128" priority="69">
+    <cfRule type="expression" dxfId="132" priority="69">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:H111 B107:H108">
-    <cfRule type="expression" dxfId="127" priority="61">
+    <cfRule type="expression" dxfId="131" priority="61">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:H111 B107:H108">
-    <cfRule type="expression" dxfId="126" priority="62">
+    <cfRule type="expression" dxfId="130" priority="62">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D107:D111">
-    <cfRule type="expression" dxfId="125" priority="60">
+    <cfRule type="expression" dxfId="129" priority="60">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A22 A24:A108">
-    <cfRule type="expression" dxfId="124" priority="58">
+    <cfRule type="expression" dxfId="128" priority="58">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A22 A24:A108">
-    <cfRule type="expression" dxfId="123" priority="59">
+    <cfRule type="expression" dxfId="127" priority="59">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="expression" dxfId="122" priority="57">
+    <cfRule type="expression" dxfId="126" priority="57">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79:A83">
-    <cfRule type="expression" dxfId="121" priority="56">
+    <cfRule type="expression" dxfId="125" priority="56">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="120" priority="55">
+    <cfRule type="expression" dxfId="124" priority="55">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="119" priority="54">
+    <cfRule type="expression" dxfId="123" priority="54">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="118" priority="53">
+    <cfRule type="expression" dxfId="122" priority="53">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="117" priority="52">
+    <cfRule type="expression" dxfId="121" priority="52">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="expression" dxfId="116" priority="51">
+    <cfRule type="expression" dxfId="120" priority="51">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="115" priority="50">
+    <cfRule type="expression" dxfId="119" priority="50">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="114" priority="49">
+    <cfRule type="expression" dxfId="118" priority="49">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="113" priority="48">
+    <cfRule type="expression" dxfId="117" priority="48">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="112" priority="47">
+    <cfRule type="expression" dxfId="116" priority="47">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="111" priority="46">
+    <cfRule type="expression" dxfId="115" priority="46">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="110" priority="45">
+    <cfRule type="expression" dxfId="114" priority="45">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="109" priority="44">
+    <cfRule type="expression" dxfId="113" priority="44">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="108" priority="43">
+    <cfRule type="expression" dxfId="112" priority="43">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="107" priority="42">
+    <cfRule type="expression" dxfId="111" priority="42">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="106" priority="41">
+    <cfRule type="expression" dxfId="110" priority="41">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="105" priority="40">
+    <cfRule type="expression" dxfId="109" priority="40">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="104" priority="39">
+    <cfRule type="expression" dxfId="108" priority="39">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="103" priority="38">
+    <cfRule type="expression" dxfId="107" priority="38">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="102" priority="37">
+    <cfRule type="expression" dxfId="106" priority="37">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="101" priority="36">
+    <cfRule type="expression" dxfId="105" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="100" priority="35">
+    <cfRule type="expression" dxfId="104" priority="35">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="99" priority="34">
+    <cfRule type="expression" dxfId="103" priority="34">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106">
-    <cfRule type="expression" dxfId="98" priority="33">
+    <cfRule type="expression" dxfId="102" priority="33">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107">
-    <cfRule type="expression" dxfId="97" priority="32">
+    <cfRule type="expression" dxfId="101" priority="32">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108">
-    <cfRule type="expression" dxfId="96" priority="31">
+    <cfRule type="expression" dxfId="100" priority="31">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83">
-    <cfRule type="expression" dxfId="95" priority="30">
+    <cfRule type="expression" dxfId="99" priority="30">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="94" priority="29">
+    <cfRule type="expression" dxfId="98" priority="29">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="93" priority="28">
+    <cfRule type="expression" dxfId="97" priority="28">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="92" priority="27">
+    <cfRule type="expression" dxfId="96" priority="27">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="91" priority="26">
+    <cfRule type="expression" dxfId="95" priority="26">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="90" priority="25">
+    <cfRule type="expression" dxfId="94" priority="25">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="89" priority="24">
+    <cfRule type="expression" dxfId="93" priority="24">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="88" priority="23">
+    <cfRule type="expression" dxfId="92" priority="23">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="87" priority="22">
+    <cfRule type="expression" dxfId="91" priority="22">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="86" priority="21">
+    <cfRule type="expression" dxfId="90" priority="21">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="85" priority="20">
+    <cfRule type="expression" dxfId="89" priority="20">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="84" priority="19">
+    <cfRule type="expression" dxfId="88" priority="19">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="83" priority="18">
+    <cfRule type="expression" dxfId="87" priority="18">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="82" priority="17">
+    <cfRule type="expression" dxfId="86" priority="17">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="81" priority="16">
+    <cfRule type="expression" dxfId="85" priority="16">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="80" priority="15">
+    <cfRule type="expression" dxfId="84" priority="15">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="79" priority="14">
+    <cfRule type="expression" dxfId="83" priority="14">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="78" priority="13">
+    <cfRule type="expression" dxfId="82" priority="13">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="77" priority="12">
+    <cfRule type="expression" dxfId="81" priority="12">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="76" priority="11">
+    <cfRule type="expression" dxfId="80" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="75" priority="10">
+    <cfRule type="expression" dxfId="79" priority="10">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="74" priority="9">
+    <cfRule type="expression" dxfId="78" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="73" priority="8">
+    <cfRule type="expression" dxfId="77" priority="8">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="72" priority="7">
+    <cfRule type="expression" dxfId="76" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="71" priority="6">
+    <cfRule type="expression" dxfId="75" priority="6">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="70" priority="5">
+    <cfRule type="expression" dxfId="74" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="69" priority="4">
+    <cfRule type="expression" dxfId="73" priority="4">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="68" priority="3">
+    <cfRule type="expression" dxfId="72" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="67" priority="1">
+    <cfRule type="expression" dxfId="71" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="66" priority="2">
+    <cfRule type="expression" dxfId="70" priority="2">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19334,336 +19360,336 @@
       <c r="B121" s="34"/>
     </row>
   </sheetData>
-  <sortState ref="A2:C108">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C108">
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A112:C121 A109:B111 B2:C80 B106:C116 C81:C110 B82:B108">
-    <cfRule type="expression" dxfId="65" priority="79">
+    <cfRule type="expression" dxfId="69" priority="79">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1 A112:C121 A109:B111 C81:C111 B82:B108 B2:C80">
-    <cfRule type="expression" dxfId="64" priority="80">
+    <cfRule type="expression" dxfId="68" priority="80">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A112">
-    <cfRule type="expression" dxfId="63" priority="67">
+    <cfRule type="expression" dxfId="67" priority="67">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A113">
-    <cfRule type="expression" dxfId="62" priority="66">
+    <cfRule type="expression" dxfId="66" priority="66">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114">
-    <cfRule type="expression" dxfId="61" priority="65">
+    <cfRule type="expression" dxfId="65" priority="65">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A115">
-    <cfRule type="expression" dxfId="60" priority="64">
+    <cfRule type="expression" dxfId="64" priority="64">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116">
-    <cfRule type="expression" dxfId="59" priority="63">
+    <cfRule type="expression" dxfId="63" priority="63">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81">
-    <cfRule type="expression" dxfId="58" priority="59">
+    <cfRule type="expression" dxfId="62" priority="59">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81">
-    <cfRule type="expression" dxfId="57" priority="60">
+    <cfRule type="expression" dxfId="61" priority="60">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A108">
-    <cfRule type="expression" dxfId="56" priority="56">
+    <cfRule type="expression" dxfId="60" priority="56">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A108">
-    <cfRule type="expression" dxfId="55" priority="57">
+    <cfRule type="expression" dxfId="59" priority="57">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="expression" dxfId="54" priority="55">
+    <cfRule type="expression" dxfId="58" priority="55">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79:A83">
-    <cfRule type="expression" dxfId="53" priority="54">
+    <cfRule type="expression" dxfId="57" priority="54">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="52" priority="53">
+    <cfRule type="expression" dxfId="56" priority="53">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="51" priority="52">
+    <cfRule type="expression" dxfId="55" priority="52">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="50" priority="51">
+    <cfRule type="expression" dxfId="54" priority="51">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="49" priority="50">
+    <cfRule type="expression" dxfId="53" priority="50">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="expression" dxfId="48" priority="49">
+    <cfRule type="expression" dxfId="52" priority="49">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="47" priority="48">
+    <cfRule type="expression" dxfId="51" priority="48">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="46" priority="47">
+    <cfRule type="expression" dxfId="50" priority="47">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="45" priority="46">
+    <cfRule type="expression" dxfId="49" priority="46">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="44" priority="45">
+    <cfRule type="expression" dxfId="48" priority="45">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="43" priority="44">
+    <cfRule type="expression" dxfId="47" priority="44">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="42" priority="43">
+    <cfRule type="expression" dxfId="46" priority="43">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="41" priority="42">
+    <cfRule type="expression" dxfId="45" priority="42">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="40" priority="41">
+    <cfRule type="expression" dxfId="44" priority="41">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="39" priority="40">
+    <cfRule type="expression" dxfId="43" priority="40">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="42" priority="39">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="37" priority="38">
+    <cfRule type="expression" dxfId="41" priority="38">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="36" priority="37">
+    <cfRule type="expression" dxfId="40" priority="37">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="39" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="38" priority="35">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="33" priority="34">
+    <cfRule type="expression" dxfId="37" priority="34">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="36" priority="33">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="35" priority="32">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106">
-    <cfRule type="expression" dxfId="30" priority="31">
+    <cfRule type="expression" dxfId="34" priority="31">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107">
-    <cfRule type="expression" dxfId="29" priority="30">
+    <cfRule type="expression" dxfId="33" priority="30">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108">
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="32" priority="29">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83">
-    <cfRule type="expression" dxfId="27" priority="28">
+    <cfRule type="expression" dxfId="31" priority="28">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="30" priority="27">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="29" priority="26">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="24" priority="25">
+    <cfRule type="expression" dxfId="28" priority="25">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="23" priority="24">
+    <cfRule type="expression" dxfId="27" priority="24">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="26" priority="23">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="25" priority="22">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="24" priority="21">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="23" priority="20">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="22" priority="19">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="21" priority="18">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="20" priority="17">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="19" priority="16">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="18" priority="15">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="17" priority="14">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="16" priority="13">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="14" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="13" priority="10">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19697,7 +19723,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <f ca="1">NOW()</f>
-        <v>45092.618308912039</v>
+        <v>45093.708055555559</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added config for ISPEnergy & Capaciy Offers
</commit_message>
<xml_diff>
--- a/src/exso/Files/ReportsInfo.xlsx
+++ b/src/exso/Files/ReportsInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.natsikas\Desktop\Admie-Desktop\exso\src\exso\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B47CEA3-3FB3-4B40-AE0D-49E0AFC096E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D692FB-E96E-44E3-9171-81AC326017C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1150,7 +1150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="314">
   <si>
     <t>AdhocISPResults</t>
   </si>
@@ -2093,6 +2093,9 @@
   </si>
   <si>
     <t>ISPResults.csv</t>
+  </si>
+  <si>
+    <t>['ISPCapacityOffers']</t>
   </si>
 </sst>
 </file>
@@ -2676,6 +2679,391 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -2739,356 +3127,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -3152,6 +3190,356 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -3166,6 +3554,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -3180,391 +3575,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -3579,13 +3589,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -3628,6 +3631,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
@@ -3643,13 +3653,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6642,8 +6645,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71:D72"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8985,8 +8988,7 @@
         <v>1</v>
       </c>
       <c r="I77" s="1" t="b">
-        <f>IF(Metadata!G77="",TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J77" s="37" t="s">
         <v>82</v>
@@ -9005,7 +9007,7 @@
         <v>308</v>
       </c>
       <c r="E78" s="18">
-        <v>44136</v>
+        <v>44221</v>
       </c>
       <c r="F78" s="13"/>
       <c r="G78" s="22" t="b">
@@ -9016,7 +9018,7 @@
         <v>1</v>
       </c>
       <c r="I78" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78" s="37" t="s">
         <v>82</v>
@@ -10834,8 +10836,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12321,9 +12323,15 @@
       </c>
       <c r="C77" s="22"/>
       <c r="D77" s="21"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="22"/>
-      <c r="G77" s="6"/>
+      <c r="E77" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F77" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="G77" s="6">
+        <v>0</v>
+      </c>
       <c r="H77" s="6"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -13402,8 +13410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D990D66-1D5A-4927-9AF4-58A372472D57}">
   <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14648,9 +14656,15 @@
       <c r="C77" s="38"/>
       <c r="D77" s="22"/>
       <c r="E77" s="22"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="28"/>
-      <c r="H77" s="9"/>
+      <c r="F77" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G77" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H77" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
@@ -15710,22 +15724,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="142" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="141" priority="4">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="140" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="139" priority="2">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15739,8 +15753,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17368,7 +17382,9 @@
         <v>126</v>
       </c>
       <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
+      <c r="E77" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="F77" s="6">
         <v>0</v>
       </c>
@@ -17980,367 +17996,367 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A112:H115 B2:H79 B82:H106">
-    <cfRule type="expression" dxfId="142" priority="117">
+    <cfRule type="expression" dxfId="138" priority="117">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:H1 A112:H115 B2:H79 B82:H106">
-    <cfRule type="expression" dxfId="141" priority="118">
+    <cfRule type="expression" dxfId="137" priority="118">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="expression" dxfId="140" priority="83">
+    <cfRule type="expression" dxfId="136" priority="83">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:H80">
-    <cfRule type="expression" dxfId="139" priority="77">
+    <cfRule type="expression" dxfId="135" priority="77">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:H80">
-    <cfRule type="expression" dxfId="138" priority="78">
+    <cfRule type="expression" dxfId="134" priority="78">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81:F81 H81">
-    <cfRule type="expression" dxfId="137" priority="72">
+    <cfRule type="expression" dxfId="133" priority="72">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81:F81 H81">
-    <cfRule type="expression" dxfId="136" priority="73">
+    <cfRule type="expression" dxfId="132" priority="73">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81:C81">
-    <cfRule type="expression" dxfId="135" priority="70">
+    <cfRule type="expression" dxfId="131" priority="70">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81:C81">
-    <cfRule type="expression" dxfId="134" priority="71">
+    <cfRule type="expression" dxfId="130" priority="71">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81">
-    <cfRule type="expression" dxfId="133" priority="68">
+    <cfRule type="expression" dxfId="129" priority="68">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81">
-    <cfRule type="expression" dxfId="132" priority="69">
+    <cfRule type="expression" dxfId="128" priority="69">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:H111 B107:H108">
-    <cfRule type="expression" dxfId="131" priority="61">
+    <cfRule type="expression" dxfId="127" priority="61">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:H111 B107:H108">
-    <cfRule type="expression" dxfId="130" priority="62">
+    <cfRule type="expression" dxfId="126" priority="62">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D107:D111">
-    <cfRule type="expression" dxfId="129" priority="60">
+    <cfRule type="expression" dxfId="125" priority="60">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A22 A24:A108">
-    <cfRule type="expression" dxfId="128" priority="58">
+    <cfRule type="expression" dxfId="124" priority="58">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A22 A24:A108">
-    <cfRule type="expression" dxfId="127" priority="59">
+    <cfRule type="expression" dxfId="123" priority="59">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="expression" dxfId="126" priority="57">
+    <cfRule type="expression" dxfId="122" priority="57">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79:A83">
-    <cfRule type="expression" dxfId="125" priority="56">
+    <cfRule type="expression" dxfId="121" priority="56">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="124" priority="55">
+    <cfRule type="expression" dxfId="120" priority="55">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="123" priority="54">
+    <cfRule type="expression" dxfId="119" priority="54">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="122" priority="53">
+    <cfRule type="expression" dxfId="118" priority="53">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="121" priority="52">
+    <cfRule type="expression" dxfId="117" priority="52">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="expression" dxfId="120" priority="51">
+    <cfRule type="expression" dxfId="116" priority="51">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="119" priority="50">
+    <cfRule type="expression" dxfId="115" priority="50">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="118" priority="49">
+    <cfRule type="expression" dxfId="114" priority="49">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="117" priority="48">
+    <cfRule type="expression" dxfId="113" priority="48">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="116" priority="47">
+    <cfRule type="expression" dxfId="112" priority="47">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="115" priority="46">
+    <cfRule type="expression" dxfId="111" priority="46">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="114" priority="45">
+    <cfRule type="expression" dxfId="110" priority="45">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="113" priority="44">
+    <cfRule type="expression" dxfId="109" priority="44">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="112" priority="43">
+    <cfRule type="expression" dxfId="108" priority="43">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="111" priority="42">
+    <cfRule type="expression" dxfId="107" priority="42">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="110" priority="41">
+    <cfRule type="expression" dxfId="106" priority="41">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="109" priority="40">
+    <cfRule type="expression" dxfId="105" priority="40">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="108" priority="39">
+    <cfRule type="expression" dxfId="104" priority="39">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="107" priority="38">
+    <cfRule type="expression" dxfId="103" priority="38">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="106" priority="37">
+    <cfRule type="expression" dxfId="102" priority="37">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="105" priority="36">
+    <cfRule type="expression" dxfId="101" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="104" priority="35">
+    <cfRule type="expression" dxfId="100" priority="35">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="103" priority="34">
+    <cfRule type="expression" dxfId="99" priority="34">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106">
-    <cfRule type="expression" dxfId="102" priority="33">
+    <cfRule type="expression" dxfId="98" priority="33">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107">
-    <cfRule type="expression" dxfId="101" priority="32">
+    <cfRule type="expression" dxfId="97" priority="32">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108">
-    <cfRule type="expression" dxfId="100" priority="31">
+    <cfRule type="expression" dxfId="96" priority="31">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83">
-    <cfRule type="expression" dxfId="99" priority="30">
+    <cfRule type="expression" dxfId="95" priority="30">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="98" priority="29">
+    <cfRule type="expression" dxfId="94" priority="29">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="97" priority="28">
+    <cfRule type="expression" dxfId="93" priority="28">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="96" priority="27">
+    <cfRule type="expression" dxfId="92" priority="27">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="95" priority="26">
+    <cfRule type="expression" dxfId="91" priority="26">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="94" priority="25">
+    <cfRule type="expression" dxfId="90" priority="25">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="93" priority="24">
+    <cfRule type="expression" dxfId="89" priority="24">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="92" priority="23">
+    <cfRule type="expression" dxfId="88" priority="23">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="91" priority="22">
+    <cfRule type="expression" dxfId="87" priority="22">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="90" priority="21">
+    <cfRule type="expression" dxfId="86" priority="21">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="89" priority="20">
+    <cfRule type="expression" dxfId="85" priority="20">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="88" priority="19">
+    <cfRule type="expression" dxfId="84" priority="19">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="87" priority="18">
+    <cfRule type="expression" dxfId="83" priority="18">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="86" priority="17">
+    <cfRule type="expression" dxfId="82" priority="17">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="85" priority="16">
+    <cfRule type="expression" dxfId="81" priority="16">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="84" priority="15">
+    <cfRule type="expression" dxfId="80" priority="15">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="83" priority="14">
+    <cfRule type="expression" dxfId="79" priority="14">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="82" priority="13">
+    <cfRule type="expression" dxfId="78" priority="13">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="81" priority="12">
+    <cfRule type="expression" dxfId="77" priority="12">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="80" priority="11">
+    <cfRule type="expression" dxfId="76" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="79" priority="10">
+    <cfRule type="expression" dxfId="75" priority="10">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="78" priority="9">
+    <cfRule type="expression" dxfId="74" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="77" priority="8">
+    <cfRule type="expression" dxfId="73" priority="8">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="76" priority="7">
+    <cfRule type="expression" dxfId="72" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="75" priority="6">
+    <cfRule type="expression" dxfId="71" priority="6">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="74" priority="5">
+    <cfRule type="expression" dxfId="70" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="73" priority="4">
+    <cfRule type="expression" dxfId="69" priority="4">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="72" priority="3">
+    <cfRule type="expression" dxfId="68" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="71" priority="1">
+    <cfRule type="expression" dxfId="67" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="70" priority="2">
+    <cfRule type="expression" dxfId="66" priority="2">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19364,332 +19380,332 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A112:C121 A109:B111 B2:C80 B106:C116 C81:C110 B82:B108">
-    <cfRule type="expression" dxfId="69" priority="79">
+    <cfRule type="expression" dxfId="65" priority="79">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1 A112:C121 A109:B111 C81:C111 B82:B108 B2:C80">
-    <cfRule type="expression" dxfId="68" priority="80">
+    <cfRule type="expression" dxfId="64" priority="80">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A112">
-    <cfRule type="expression" dxfId="67" priority="67">
+    <cfRule type="expression" dxfId="63" priority="67">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A113">
-    <cfRule type="expression" dxfId="66" priority="66">
+    <cfRule type="expression" dxfId="62" priority="66">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114">
-    <cfRule type="expression" dxfId="65" priority="65">
+    <cfRule type="expression" dxfId="61" priority="65">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A115">
-    <cfRule type="expression" dxfId="64" priority="64">
+    <cfRule type="expression" dxfId="60" priority="64">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116">
-    <cfRule type="expression" dxfId="63" priority="63">
+    <cfRule type="expression" dxfId="59" priority="63">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81">
-    <cfRule type="expression" dxfId="62" priority="59">
+    <cfRule type="expression" dxfId="58" priority="59">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81">
-    <cfRule type="expression" dxfId="61" priority="60">
+    <cfRule type="expression" dxfId="57" priority="60">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A108">
-    <cfRule type="expression" dxfId="60" priority="56">
+    <cfRule type="expression" dxfId="56" priority="56">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A108">
-    <cfRule type="expression" dxfId="59" priority="57">
+    <cfRule type="expression" dxfId="55" priority="57">
       <formula>COLUMN()=CELL("col")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="expression" dxfId="58" priority="55">
+    <cfRule type="expression" dxfId="54" priority="55">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79:A83">
-    <cfRule type="expression" dxfId="57" priority="54">
+    <cfRule type="expression" dxfId="53" priority="54">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="56" priority="53">
+    <cfRule type="expression" dxfId="52" priority="53">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="55" priority="52">
+    <cfRule type="expression" dxfId="51" priority="52">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="54" priority="51">
+    <cfRule type="expression" dxfId="50" priority="51">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="53" priority="50">
+    <cfRule type="expression" dxfId="49" priority="50">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="expression" dxfId="52" priority="49">
+    <cfRule type="expression" dxfId="48" priority="49">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="51" priority="48">
+    <cfRule type="expression" dxfId="47" priority="48">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="50" priority="47">
+    <cfRule type="expression" dxfId="46" priority="47">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="49" priority="46">
+    <cfRule type="expression" dxfId="45" priority="46">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="48" priority="45">
+    <cfRule type="expression" dxfId="44" priority="45">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="47" priority="44">
+    <cfRule type="expression" dxfId="43" priority="44">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="46" priority="43">
+    <cfRule type="expression" dxfId="42" priority="43">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="45" priority="42">
+    <cfRule type="expression" dxfId="41" priority="42">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="44" priority="41">
+    <cfRule type="expression" dxfId="40" priority="41">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="43" priority="40">
+    <cfRule type="expression" dxfId="39" priority="40">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="42" priority="39">
+    <cfRule type="expression" dxfId="38" priority="39">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="41" priority="38">
+    <cfRule type="expression" dxfId="37" priority="38">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="40" priority="37">
+    <cfRule type="expression" dxfId="36" priority="37">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="39" priority="36">
+    <cfRule type="expression" dxfId="35" priority="36">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="38" priority="35">
+    <cfRule type="expression" dxfId="34" priority="35">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="37" priority="34">
+    <cfRule type="expression" dxfId="33" priority="34">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="36" priority="33">
+    <cfRule type="expression" dxfId="32" priority="33">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="35" priority="32">
+    <cfRule type="expression" dxfId="31" priority="32">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106">
-    <cfRule type="expression" dxfId="34" priority="31">
+    <cfRule type="expression" dxfId="30" priority="31">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107">
-    <cfRule type="expression" dxfId="33" priority="30">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108">
-    <cfRule type="expression" dxfId="32" priority="29">
+    <cfRule type="expression" dxfId="28" priority="29">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83">
-    <cfRule type="expression" dxfId="31" priority="28">
+    <cfRule type="expression" dxfId="27" priority="28">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="30" priority="27">
+    <cfRule type="expression" dxfId="26" priority="27">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="29" priority="26">
+    <cfRule type="expression" dxfId="25" priority="26">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="28" priority="25">
+    <cfRule type="expression" dxfId="24" priority="25">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="27" priority="24">
+    <cfRule type="expression" dxfId="23" priority="24">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="26" priority="23">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90">
-    <cfRule type="expression" dxfId="25" priority="22">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="24" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="expression" dxfId="23" priority="20">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="expression" dxfId="22" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="expression" dxfId="21" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="20" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="19" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="expression" dxfId="18" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="17" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="16" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="15" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="14" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="13" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="11" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="expression" dxfId="9" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A104">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19723,7 +19739,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <f ca="1">NOW()</f>
-        <v>45093.708055555559</v>
+        <v>45113.518726851849</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>